<commit_message>
change mysql connection by durid connection pool
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/btreemysqlcases/dql/casegroup1/mysql_dql_cases1_btree.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/btreemysqlcases/dql/casegroup1/mysql_dql_cases1_btree.xlsx
@@ -21195,8 +21195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1796"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1765" workbookViewId="0">
-      <selection activeCell="C1800" sqref="C1800"/>
+    <sheetView tabSelected="1" topLeftCell="A1594" workbookViewId="0">
+      <selection activeCell="C1613" sqref="C1613"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -66203,7 +66203,7 @@
         <v>5022</v>
       </c>
       <c r="B1609" s="8" t="s">
-        <v>34</v>
+        <v>2906</v>
       </c>
       <c r="C1609" s="1" t="s">
         <v>3003</v>

</xml_diff>